<commit_message>
Figured out how to get science values working - now I just need to reapply it to all the rest...
</commit_message>
<xml_diff>
--- a/Plotting/0.9.0/PlanetScienceClasses.xlsx
+++ b/Plotting/0.9.0/PlanetScienceClasses.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\Steam\steamapps\common\Kerbal Space Program\GameData\SkyhawkScienceSystem\Plotting\0.9.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50494039-D50D-4749-A70A-68E18DA9A057}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAF9F536-2210-4E23-8461-C7E49C8E282A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="-7368" yWindow="1368" windowWidth="15228" windowHeight="11232" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2256" yWindow="1488" windowWidth="15228" windowHeight="11232" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Default" sheetId="8" r:id="rId1"/>
@@ -32,29 +32,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>Science Class</t>
   </si>
   <si>
-    <t>Surface</t>
-  </si>
-  <si>
-    <t>Flying Low</t>
-  </si>
-  <si>
-    <t>Flying High</t>
-  </si>
-  <si>
-    <t>Space Low</t>
-  </si>
-  <si>
-    <t>Space High</t>
-  </si>
-  <si>
-    <t>Recovery</t>
-  </si>
-  <si>
     <t>Kerbin</t>
   </si>
   <si>
@@ -71,6 +53,57 @@
   </si>
   <si>
     <t>*Moons are assumed to be in same class unless otherwise listed</t>
+  </si>
+  <si>
+    <t>Dres</t>
+  </si>
+  <si>
+    <t>Jool</t>
+  </si>
+  <si>
+    <t>Eeloo</t>
+  </si>
+  <si>
+    <t>Homeworld</t>
+  </si>
+  <si>
+    <t>Homeworld Moons</t>
+  </si>
+  <si>
+    <t>Inner Planets</t>
+  </si>
+  <si>
+    <t>Inner Kuiper Belt</t>
+  </si>
+  <si>
+    <t>Urlum</t>
+  </si>
+  <si>
+    <t>Neidon</t>
+  </si>
+  <si>
+    <t>Sarnus</t>
+  </si>
+  <si>
+    <t>Outer Scattered Disc</t>
+  </si>
+  <si>
+    <t>Inner Scattered Disc</t>
+  </si>
+  <si>
+    <t>Inner Belt and Moho</t>
+  </si>
+  <si>
+    <t>Outer Belt and far-inner planets</t>
+  </si>
+  <si>
+    <t>Outer Kuiper Belt</t>
+  </si>
+  <si>
+    <t>Deep Space</t>
+  </si>
+  <si>
+    <t>Extra .5 each for high inclination or wacky orbits (comets esp)</t>
   </si>
 </sst>
 </file>
@@ -388,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1C83F10-F0CC-452C-89DD-D3975DD6A483}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -399,76 +432,128 @@
     <col min="1" max="1" width="11.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
+        <v>4.5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7">
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>5.5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8">
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>6.5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9">
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>7.5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10">
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>8.5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11">
+      <c r="B15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16">
         <v>10</v>
       </c>
     </row>
@@ -481,8 +566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -495,7 +580,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -503,7 +588,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -511,10 +596,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -522,25 +607,34 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>